<commit_message>
prepared to add irregular verbs, other minor improvements
</commit_message>
<xml_diff>
--- a/german_verbs.xlsx
+++ b/german_verbs.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brgubo\OneDrive - Chr Hansen\Documents\Spain\statistics\german\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Projects\deutche_verben_game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="8_{1213731F-552E-4DBC-BDF8-2F21FA900B54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{46EA293A-374F-4937-A9AA-93093BF8056B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA6FD85-4659-4C28-8A9E-26C4B56321A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{77EB7350-CF8E-467E-91F5-DE8D003E4FED}"/>
+    <workbookView xWindow="21490" yWindow="-15270" windowWidth="38620" windowHeight="21220" xr2:uid="{77EB7350-CF8E-467E-91F5-DE8D003E4FED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="regular" sheetId="1" r:id="rId1"/>
+    <sheet name="irregular" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="80">
   <si>
     <t>Verb</t>
   </si>
@@ -141,9 +142,6 @@
   </si>
   <si>
     <t>heisst</t>
-  </si>
-  <si>
-    <t>heist</t>
   </si>
   <si>
     <t>kaufen</t>
@@ -630,12 +628,12 @@
   <dimension ref="A1:C103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -646,7 +644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -657,7 +655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -668,7 +666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -679,7 +677,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -690,7 +688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -701,7 +699,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -712,7 +710,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -723,7 +721,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -734,7 +732,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -745,7 +743,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -756,7 +754,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -767,7 +765,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -778,7 +776,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -789,7 +787,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -800,7 +798,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -811,7 +809,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -822,7 +820,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -833,7 +831,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -844,7 +842,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -855,7 +853,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -866,7 +864,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -877,7 +875,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -888,7 +886,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -899,7 +897,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -910,7 +908,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -921,7 +919,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -932,7 +930,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -943,7 +941,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -954,7 +952,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -965,7 +963,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -976,7 +974,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -987,7 +985,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -998,7 +996,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1009,7 +1007,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1020,7 +1018,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -1028,10 +1026,10 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -1042,733 +1040,747 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41" t="s">
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B44" t="s">
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45" t="s">
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B46" t="s">
         <v>14</v>
       </c>
       <c r="C46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" t="s">
         <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49" t="s">
         <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B51" t="s">
         <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B52" t="s">
         <v>14</v>
       </c>
       <c r="C52" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B53" t="s">
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B54" t="s">
         <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B55" t="s">
         <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B56" t="s">
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B57" t="s">
         <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B58" t="s">
         <v>14</v>
       </c>
       <c r="C58" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>52</v>
       </c>
       <c r="B59" t="s">
         <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B60" t="s">
         <v>4</v>
       </c>
       <c r="C60" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>52</v>
       </c>
       <c r="B61" t="s">
         <v>5</v>
       </c>
       <c r="C61" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>53</v>
       </c>
       <c r="B62" t="s">
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B63" t="s">
         <v>2</v>
       </c>
       <c r="C63" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B64" t="s">
         <v>14</v>
       </c>
       <c r="C64" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B65" t="s">
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B66" t="s">
         <v>4</v>
       </c>
       <c r="C66" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B67" t="s">
         <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B68" t="s">
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B69" t="s">
         <v>2</v>
       </c>
       <c r="C69" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B70" t="s">
         <v>14</v>
       </c>
       <c r="C70" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B71" t="s">
         <v>3</v>
       </c>
       <c r="C71" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B72" t="s">
         <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B73" t="s">
         <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B74" t="s">
         <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B75" t="s">
         <v>2</v>
       </c>
       <c r="C75" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B76" t="s">
         <v>14</v>
       </c>
       <c r="C76" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B77" t="s">
         <v>3</v>
       </c>
       <c r="C77" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B78" t="s">
         <v>4</v>
       </c>
       <c r="C78" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B79" t="s">
         <v>5</v>
       </c>
       <c r="C79" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B80" t="s">
         <v>1</v>
       </c>
       <c r="C80" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B81" t="s">
         <v>2</v>
       </c>
       <c r="C81" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B82" t="s">
         <v>14</v>
       </c>
       <c r="C82" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B83" t="s">
         <v>3</v>
       </c>
       <c r="C83" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B84" t="s">
         <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B85" t="s">
         <v>5</v>
       </c>
       <c r="C85" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B86" t="s">
         <v>1</v>
       </c>
       <c r="C86" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B87" t="s">
         <v>2</v>
       </c>
       <c r="C87" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B88" t="s">
         <v>14</v>
       </c>
       <c r="C88" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B89" t="s">
         <v>3</v>
       </c>
       <c r="C89" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B90" t="s">
         <v>4</v>
       </c>
       <c r="C90" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B91" t="s">
         <v>5</v>
       </c>
       <c r="C91" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B92" t="s">
         <v>1</v>
       </c>
       <c r="C92" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B93" t="s">
         <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B94" t="s">
         <v>14</v>
       </c>
       <c r="C94" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B95" t="s">
         <v>3</v>
       </c>
       <c r="C95" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B96" t="s">
         <v>4</v>
       </c>
       <c r="C96" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B97" t="s">
         <v>5</v>
       </c>
       <c r="C97" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B98" t="s">
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B99" t="s">
         <v>2</v>
       </c>
       <c r="C99" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B100" t="s">
         <v>14</v>
       </c>
       <c r="C100" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B101" t="s">
         <v>3</v>
       </c>
       <c r="C101" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B102" t="s">
         <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B103" t="s">
         <v>5</v>
       </c>
       <c r="C103" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD6761C-4478-4365-AAA2-59BFE402FE28}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>